<commit_message>
Added the standardization function in the cleaning process.
</commit_message>
<xml_diff>
--- a/Test_data.xlsx
+++ b/Test_data.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siddhaant Pahuja\codes\EDA_tool\EDA_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24E075F-236E-4F6C-93AA-A6C6035E32AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD4A250-7543-47BC-9FF0-96B94AE19074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$22</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -112,6 +115,126 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Audi</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>Lexus</t>
+  </si>
+  <si>
+    <t>AUDI</t>
+  </si>
+  <si>
+    <t>bmw</t>
+  </si>
+  <si>
+    <t>Mer</t>
+  </si>
+  <si>
+    <t>Lxs</t>
+  </si>
+  <si>
+    <t>mercedes</t>
+  </si>
+  <si>
+    <t>riggs Navarro</t>
+  </si>
+  <si>
+    <t>Winter Browning</t>
+  </si>
+  <si>
+    <t>Rohan Phan</t>
+  </si>
+  <si>
+    <t>Elsa Mendoza</t>
+  </si>
+  <si>
+    <t>Dominic Weber</t>
+  </si>
+  <si>
+    <t>Alayah Johnson</t>
+  </si>
+  <si>
+    <t>Noah Fry</t>
+  </si>
+  <si>
+    <t>Clarissa Ross</t>
+  </si>
+  <si>
+    <t>Wesley Shannon</t>
+  </si>
+  <si>
+    <t>Harlee Chavez</t>
+  </si>
+  <si>
+    <t>Ian Bailey</t>
+  </si>
+  <si>
+    <t>Kennedy Hines</t>
+  </si>
+  <si>
+    <t>Uriel Jarvis</t>
+  </si>
+  <si>
+    <t>Elisabeth Stark</t>
+  </si>
+  <si>
+    <t>Kristopher Khan</t>
+  </si>
+  <si>
+    <t>Mabel Yoder</t>
+  </si>
+  <si>
+    <t>Johan Beltran</t>
+  </si>
+  <si>
+    <t>Kaydence Jacobs</t>
+  </si>
+  <si>
+    <t>Bryan Miller</t>
+  </si>
+  <si>
+    <t>Isabella Cameron</t>
+  </si>
+  <si>
+    <t>Rayan Elliott</t>
+  </si>
+  <si>
+    <t>Noelle Espinoza</t>
+  </si>
+  <si>
+    <t>Dallas Avila</t>
+  </si>
+  <si>
+    <t>Amiyah Ross</t>
+  </si>
+  <si>
+    <t>Wesley Garner</t>
+  </si>
+  <si>
+    <t>Jacqueline Kent</t>
+  </si>
+  <si>
+    <t>Mekhi Holland</t>
+  </si>
+  <si>
+    <t>Mariah Garza</t>
+  </si>
+  <si>
+    <t>Judah Mejia</t>
+  </si>
+  <si>
+    <t>Saylor Hayden</t>
   </si>
 </sst>
 </file>
@@ -429,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,7 +563,7 @@
     <col min="2" max="2" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -456,8 +579,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -473,8 +599,11 @@
       <c r="E2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -490,8 +619,11 @@
       <c r="E3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1002</v>
       </c>
@@ -507,8 +639,11 @@
       <c r="E4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1003</v>
       </c>
@@ -524,8 +659,11 @@
       <c r="E5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1004</v>
       </c>
@@ -538,8 +676,11 @@
       <c r="E6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1005</v>
       </c>
@@ -555,8 +696,11 @@
       <c r="E7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1006</v>
       </c>
@@ -572,8 +716,11 @@
       <c r="E8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1007</v>
       </c>
@@ -586,8 +733,11 @@
       <c r="E9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1008</v>
       </c>
@@ -603,8 +753,11 @@
       <c r="E10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1009</v>
       </c>
@@ -620,8 +773,11 @@
       <c r="E11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1010</v>
       </c>
@@ -637,8 +793,11 @@
       <c r="E12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1011</v>
       </c>
@@ -654,8 +813,11 @@
       <c r="E13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1012</v>
       </c>
@@ -671,8 +833,11 @@
       <c r="E14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1013</v>
       </c>
@@ -685,8 +850,11 @@
       <c r="D15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1014</v>
       </c>
@@ -702,8 +870,11 @@
       <c r="E16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1015</v>
       </c>
@@ -719,8 +890,11 @@
       <c r="E17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1016</v>
       </c>
@@ -736,8 +910,11 @@
       <c r="E18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1017</v>
       </c>
@@ -753,8 +930,11 @@
       <c r="E19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1018</v>
       </c>
@@ -770,8 +950,11 @@
       <c r="E20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1019</v>
       </c>
@@ -787,8 +970,11 @@
       <c r="E21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1020</v>
       </c>
@@ -804,8 +990,613 @@
       <c r="E22" t="s">
         <v>25</v>
       </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1021</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1022</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>1023</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1024</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1025</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1026</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28">
+        <v>36</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>1027</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1028</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1029</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31">
+        <v>24</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1030</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32">
+        <v>45</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>1031</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>1032</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>1033</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35">
+        <v>33</v>
+      </c>
+      <c r="D35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1034</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1035</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37">
+        <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>1036</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>1037</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39">
+        <v>35</v>
+      </c>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>1038</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40">
+        <v>35</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>1039</v>
+      </c>
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41">
+        <v>32</v>
+      </c>
+      <c r="D41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>1040</v>
+      </c>
+      <c r="B42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42">
+        <v>22</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>1041</v>
+      </c>
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43">
+        <v>45</v>
+      </c>
+      <c r="D43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1042</v>
+      </c>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44">
+        <v>25</v>
+      </c>
+      <c r="D44" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>1043</v>
+      </c>
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45">
+        <v>26</v>
+      </c>
+      <c r="D45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>1044</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46">
+        <v>47</v>
+      </c>
+      <c r="D46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1045</v>
+      </c>
+      <c r="B47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47">
+        <v>43</v>
+      </c>
+      <c r="D47" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1046</v>
+      </c>
+      <c r="B48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48">
+        <v>54</v>
+      </c>
+      <c r="D48" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1047</v>
+      </c>
+      <c r="B49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49">
+        <v>35</v>
+      </c>
+      <c r="D49" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>1048</v>
+      </c>
+      <c r="B50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50">
+        <v>35</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1049</v>
+      </c>
+      <c r="B51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>1050</v>
+      </c>
+      <c r="B52" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52">
+        <v>35</v>
+      </c>
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A22" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
+      <sortCondition ref="A1:A22"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
+    <sortCondition ref="F1:F22"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>